<commit_message>
Combined Levee and failure functions. Added Alternatives and Plans nodes to the study tree. Many updates to the importing from old fda studies. Updates to importing structures.
Former-commit-id: 2c2c1aa89edbb532ff4fcdba50579fbd57ee9409
</commit_message>
<xml_diff>
--- a/FunctionsTests/ExcelTesting/ExcelData/CoordinatesFunctionVariableYs.xlsx
+++ b/FunctionsTests/ExcelTesting/ExcelData/CoordinatesFunctionVariableYs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cody\source\Repos\flooddamageassessment\FunctionsTests\ExcelTesting\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153B3AA8-D5A4-4F1E-9F8B-D12AB29AF4A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17286E04-572F-4B32-9FC2-6C7E4504E784}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCE4BC34-26FE-4910-A787-A5AAF9B7D721}"/>
+    <workbookView minimized="1" xWindow="690" yWindow="990" windowWidth="16200" windowHeight="11385" xr2:uid="{CCE4BC34-26FE-4910-A787-A5AAF9B7D721}"/>
   </bookViews>
   <sheets>
     <sheet name="Domains" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>Linked Functions Tests</t>
   </si>
@@ -127,13 +127,28 @@
   </si>
   <si>
     <t>Max</t>
+  </si>
+  <si>
+    <t>DistVal1</t>
+  </si>
+  <si>
+    <t>DistVal2</t>
+  </si>
+  <si>
+    <t>DistVal3</t>
+  </si>
+  <si>
+    <t>DistVal4</t>
+  </si>
+  <si>
+    <t>Triangular</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +173,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -538,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54B3A445-DBF2-4DC5-9985-412C468F77F2}">
-  <dimension ref="A1:T24"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B20" sqref="B20:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,6 +571,7 @@
     <col min="3" max="3" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="10.140625" customWidth="1"/>
     <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
     <col min="12" max="12" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -715,32 +737,128 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="19:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="T17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="19:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="T18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="19:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="T19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="19:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" t="s">
+        <v>32</v>
+      </c>
+      <c r="J20" t="s">
+        <v>33</v>
+      </c>
+      <c r="K20" t="s">
+        <v>34</v>
+      </c>
+      <c r="L20" t="s">
+        <v>35</v>
+      </c>
       <c r="T20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="19:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>100</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>36</v>
+      </c>
+      <c r="I21">
+        <v>100</v>
+      </c>
+      <c r="J21">
+        <v>150</v>
+      </c>
+      <c r="K21">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="G23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="G24">
+        <v>4</v>
+      </c>
       <c r="S24" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="G25">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>